<commit_message>
Added hinge info to parts list
</commit_message>
<xml_diff>
--- a/PARTS_LIST.xlsx
+++ b/PARTS_LIST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\TR595\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1BDA09-BE43-40CE-93D9-FB04DD321D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EAA6F1-D79B-4978-A7DC-A8D04FCEC9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A83D8834-C1AC-45D0-9875-619CC4B284FE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="98">
   <si>
     <t>TR-595 Part List</t>
   </si>
@@ -319,10 +319,16 @@
     <t>PAINT</t>
   </si>
   <si>
-    <t>Duplicolor BGM0347 Medium Gray Metallic</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/1901/5629432</t>
+  </si>
+  <si>
+    <t>HINGES</t>
+  </si>
+  <si>
+    <t>STANLEY CLASSIC BRASSWARE 80-3050 3/4" (19mm)</t>
+  </si>
+  <si>
+    <t>DUPLICOLOR BGM0347 MEDIUM GRAY METALLIC</t>
   </si>
 </sst>
 </file>
@@ -706,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58EA907-1E68-4916-898D-EB0A7487479A}">
   <dimension ref="A2:P118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,7 +2324,7 @@
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
@@ -2336,7 +2342,7 @@
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
@@ -2349,7 +2355,12 @@
       <c r="L116" s="3"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="2"/>
+      <c r="A117" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C117" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>

</xml_diff>